<commit_message>
add report for assignment4
</commit_message>
<xml_diff>
--- a/report/assign4/YueFang_AssignmentNo4.xlsx
+++ b/report/assign4/YueFang_AssignmentNo4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SchoolWorks\NEU\INFO 6205\assign\INFO6205\report\assign4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1F0918-DB16-45AD-A25E-055DCF707304}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E771A48D-72FD-4C61-A867-89293C3BD0A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -460,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -536,23 +536,6 @@
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>160000</v>
-      </c>
-      <c r="C2">
-        <v>1145620</v>
-      </c>
-      <c r="D2">
-        <f t="shared" ref="D2:D8" si="0">C2/B2</f>
-        <v>7.1601249999999999</v>
-      </c>
-      <c r="E2">
-        <f t="shared" ref="E2:E26" si="1">LOG(C2,2)/LOG(B2,2)</f>
-        <v>1.1642776506013799</v>
-      </c>
       <c r="H2" t="s">
         <v>5</v>
       </c>
@@ -561,23 +544,6 @@
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>80000</v>
-      </c>
-      <c r="C3">
-        <v>466013</v>
-      </c>
-      <c r="D3">
-        <f t="shared" si="0"/>
-        <v>5.8251625000000002</v>
-      </c>
-      <c r="E3">
-        <f t="shared" si="1"/>
-        <v>1.1560868854275062</v>
-      </c>
       <c r="H3" t="s">
         <v>6</v>
       </c>
@@ -586,23 +552,6 @@
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>80000</v>
-      </c>
-      <c r="C4">
-        <v>476415</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>5.9551875000000001</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="1"/>
-        <v>1.1580422635356182</v>
-      </c>
       <c r="H4" t="s">
         <v>7</v>
       </c>
@@ -611,23 +560,6 @@
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>40000</v>
-      </c>
-      <c r="C5">
-        <v>229915</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>5.7478749999999996</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="1"/>
-        <v>1.1650363785611821</v>
-      </c>
       <c r="H5" t="s">
         <v>8</v>
       </c>
@@ -636,23 +568,6 @@
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>40000</v>
-      </c>
-      <c r="C6">
-        <v>213666</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>5.3416499999999996</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="1"/>
-        <v>1.1581195007860201</v>
-      </c>
       <c r="H6" t="s">
         <v>9</v>
       </c>
@@ -661,23 +576,6 @@
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>20000</v>
-      </c>
-      <c r="C7">
-        <v>98100</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>4.9050000000000002</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="1"/>
-        <v>1.1605752604404584</v>
-      </c>
       <c r="H7" t="s">
         <v>10</v>
       </c>
@@ -686,45 +584,11 @@
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>20000</v>
-      </c>
-      <c r="C8">
-        <v>93625</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>4.6812500000000004</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="1"/>
-        <v>1.1558607672393257</v>
-      </c>
       <c r="H8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9">
-        <v>10000</v>
-      </c>
-      <c r="C9">
-        <v>51968</v>
-      </c>
-      <c r="D9">
-        <f>C9/B9</f>
-        <v>5.1967999999999996</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="1"/>
-        <v>1.1789340008062656</v>
-      </c>
       <c r="H9" t="s">
         <v>12</v>
       </c>
@@ -733,23 +597,6 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10">
-        <v>10000</v>
-      </c>
-      <c r="C10">
-        <v>46100</v>
-      </c>
-      <c r="D10">
-        <f>C10/B10</f>
-        <v>4.6100000000000003</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="1"/>
-        <v>1.165925231347412</v>
-      </c>
       <c r="H10" t="s">
         <v>13</v>
       </c>
@@ -758,23 +605,6 @@
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11">
-        <v>5000</v>
-      </c>
-      <c r="C11">
-        <v>26633</v>
-      </c>
-      <c r="D11">
-        <f>C11/B11</f>
-        <v>5.3266</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="1"/>
-        <v>1.1963925319473707</v>
-      </c>
       <c r="H11" t="s">
         <v>14</v>
       </c>
@@ -783,45 +613,11 @@
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12">
-        <v>5000</v>
-      </c>
-      <c r="C12">
-        <v>23847</v>
-      </c>
-      <c r="D12">
-        <f t="shared" ref="D12:D26" si="2">C12/B12</f>
-        <v>4.7694000000000001</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="1"/>
-        <v>1.1834196402166168</v>
-      </c>
       <c r="H12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13">
-        <v>2500</v>
-      </c>
-      <c r="C13">
-        <v>12413</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="2"/>
-        <v>4.9652000000000003</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="1"/>
-        <v>1.2048113695185541</v>
-      </c>
       <c r="H13" t="s">
         <v>16</v>
       </c>
@@ -830,23 +626,6 @@
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14">
-        <v>1250</v>
-      </c>
-      <c r="C14">
-        <v>5947</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="2"/>
-        <v>4.7576000000000001</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="1"/>
-        <v>1.2187302577879131</v>
-      </c>
       <c r="H14" t="s">
         <v>17</v>
       </c>
@@ -855,45 +634,11 @@
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15">
-        <v>1000</v>
-      </c>
-      <c r="C15">
-        <v>3440</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="2"/>
-        <v>3.44</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="1"/>
-        <v>1.1788528141905101</v>
-      </c>
       <c r="H15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16">
-        <v>625</v>
-      </c>
-      <c r="C16">
-        <v>1813</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="2"/>
-        <v>2.9007999999999998</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="1"/>
-        <v>1.1654283387993163</v>
-      </c>
       <c r="H16" t="s">
         <v>19</v>
       </c>
@@ -904,24 +649,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17">
-        <v>500</v>
-      </c>
-      <c r="C17">
-        <v>1770</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="2"/>
-        <v>3.54</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="1"/>
-        <v>1.2034121391285524</v>
-      </c>
+    <row r="17" spans="8:23" x14ac:dyDescent="0.2">
       <c r="I17">
         <v>10</v>
       </c>
@@ -968,43 +696,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18">
-        <v>250</v>
-      </c>
-      <c r="C18">
-        <v>664</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="2"/>
-        <v>2.6560000000000001</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="1"/>
-        <v>1.1769135462779632</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19">
-        <v>125</v>
-      </c>
-      <c r="C19">
-        <v>321</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="2"/>
-        <v>2.5680000000000001</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="1"/>
-        <v>1.19533266418488</v>
-      </c>
+    <row r="19" spans="8:23" x14ac:dyDescent="0.2">
       <c r="I19">
         <v>0</v>
       </c>
@@ -1051,24 +743,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20">
-        <v>100</v>
-      </c>
-      <c r="C20">
-        <v>278</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="2"/>
-        <v>2.78</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="1"/>
-        <v>1.2220223979590379</v>
-      </c>
+    <row r="20" spans="8:23" x14ac:dyDescent="0.2">
       <c r="H20" t="s">
         <v>20</v>
       </c>
@@ -1076,24 +751,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21">
-        <v>100</v>
-      </c>
-      <c r="C21">
-        <v>224</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="2"/>
-        <v>2.2400000000000002</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="1"/>
-        <v>1.1751240091670812</v>
-      </c>
+    <row r="21" spans="8:23" x14ac:dyDescent="0.2">
       <c r="H21" t="s">
         <v>21</v>
       </c>
@@ -1101,24 +759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22">
-        <v>50</v>
-      </c>
-      <c r="C22">
-        <v>225</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="2"/>
-        <v>4.5</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="1"/>
-        <v>1.3844756011632051</v>
-      </c>
+    <row r="22" spans="8:23" x14ac:dyDescent="0.2">
       <c r="H22" t="s">
         <v>22</v>
       </c>
@@ -1126,24 +767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23">
-        <v>25</v>
-      </c>
-      <c r="C23">
-        <v>50</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="1"/>
-        <v>1.2153382790366964</v>
-      </c>
+    <row r="23" spans="8:23" x14ac:dyDescent="0.2">
       <c r="H23" t="s">
         <v>23</v>
       </c>
@@ -1151,24 +775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>2</v>
-      </c>
-      <c r="B24">
-        <v>50</v>
-      </c>
-      <c r="C24">
-        <v>80</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="2"/>
-        <v>1.6</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="1"/>
-        <v>1.1201433704744526</v>
-      </c>
+    <row r="24" spans="8:23" x14ac:dyDescent="0.2">
       <c r="H24" t="s">
         <v>24</v>
       </c>
@@ -1176,46 +783,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>2</v>
-      </c>
-      <c r="B25">
-        <v>25</v>
-      </c>
-      <c r="C25">
-        <v>58</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="2"/>
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="1"/>
-        <v>1.2614475461204464</v>
-      </c>
+    <row r="25" spans="8:23" x14ac:dyDescent="0.2">
       <c r="H25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>2</v>
-      </c>
-      <c r="B26">
-        <v>25</v>
-      </c>
-      <c r="C26">
-        <v>39</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="2"/>
-        <v>1.56</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="1"/>
-        <v>1.1381494178265339</v>
-      </c>
+    <row r="26" spans="8:23" x14ac:dyDescent="0.2">
       <c r="H26" t="s">
         <v>11</v>
       </c>
@@ -1223,12 +796,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="8:23" x14ac:dyDescent="0.2">
       <c r="H27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="8:23" x14ac:dyDescent="0.2">
       <c r="H28" t="s">
         <v>26</v>
       </c>
@@ -1236,12 +809,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="8:23" x14ac:dyDescent="0.2">
       <c r="H29" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="8:23" x14ac:dyDescent="0.2">
       <c r="H30" t="s">
         <v>27</v>
       </c>
@@ -1249,7 +822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="8:23" x14ac:dyDescent="0.2">
       <c r="H31" t="s">
         <v>28</v>
       </c>
@@ -1260,7 +833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="8:23" x14ac:dyDescent="0.2">
       <c r="H32" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
modify union method and report for assignment 4
</commit_message>
<xml_diff>
--- a/report/assign4/YueFang_AssignmentNo4.xlsx
+++ b/report/assign4/YueFang_AssignmentNo4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15620"/>
+    <workbookView windowHeight="16260"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,26 +14,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59">
-  <si>
-    <t>count</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69">
+  <si>
+    <t>WQUPC</t>
   </si>
   <si>
     <t>site (N)</t>
   </si>
   <si>
-    <t>connections (M)</t>
-  </si>
-  <si>
-    <t>ratio (connections/site)</t>
-  </si>
-  <si>
-    <t>lg ratio (log(connections, site))</t>
+    <t>time(millisecond)</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>lg ratio</t>
   </si>
   <si>
     <t>union (13, 8)</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>union (10, 11)</t>
   </si>
   <si>
@@ -76,6 +79,9 @@
     <t>union (9, 1)</t>
   </si>
   <si>
+    <t>WQU</t>
+  </si>
+  <si>
     <t>union (3, 13)</t>
   </si>
   <si>
@@ -169,28 +175,52 @@
     <t>union (4, 6)</t>
   </si>
   <si>
-    <t>union (1, 5)</t>
-  </si>
-  <si>
-    <t>union (7, 0)</t>
-  </si>
-  <si>
-    <t>union (5, 1)</t>
-  </si>
-  <si>
-    <t>union (11, 13)</t>
-  </si>
-  <si>
-    <t>union (8, 13)</t>
-  </si>
-  <si>
-    <t>union (2, 7)</t>
-  </si>
-  <si>
-    <t>union (4, 12)</t>
-  </si>
-  <si>
-    <t>union (8, 9)</t>
+    <t>union (2, 2)</t>
+  </si>
+  <si>
+    <t>union (5, 4)</t>
+  </si>
+  <si>
+    <t>union (6, 8)</t>
+  </si>
+  <si>
+    <t>union (3, 14)</t>
+  </si>
+  <si>
+    <t>union (4, 0)</t>
+  </si>
+  <si>
+    <t>union (12, 11)</t>
+  </si>
+  <si>
+    <t>union (8, 6)</t>
+  </si>
+  <si>
+    <t>union (5, 9)</t>
+  </si>
+  <si>
+    <t>union (13, 14)</t>
+  </si>
+  <si>
+    <t>union (14, 0)</t>
+  </si>
+  <si>
+    <t>union (5, 2)</t>
+  </si>
+  <si>
+    <t>union (6, 12)</t>
+  </si>
+  <si>
+    <t>union (13, 10)</t>
+  </si>
+  <si>
+    <t>union (11, 14)</t>
+  </si>
+  <si>
+    <t>union (5, 7)</t>
+  </si>
+  <si>
+    <t>union (6, 1)</t>
   </si>
 </sst>
 </file>
@@ -1132,198 +1162,354 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:W78"/>
+  <dimension ref="A1:V88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63:W63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="3" max="3" width="11.625" customWidth="1"/>
-    <col min="4" max="4" width="21.875" customWidth="1"/>
-    <col min="5" max="5" width="26.25" customWidth="1"/>
-    <col min="8" max="8" width="11.75" customWidth="1"/>
-    <col min="9" max="23" width="3.125" customWidth="1"/>
+    <col min="1" max="1" width="9.5"/>
+    <col min="2" max="2" width="14.0625" customWidth="1"/>
+    <col min="3" max="3" width="6.640625" customWidth="1"/>
+    <col min="4" max="4" width="9.625" customWidth="1"/>
+    <col min="7" max="7" width="11.75" customWidth="1"/>
+    <col min="8" max="22" width="3.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="H1">
+        <v>0</v>
+      </c>
+      <c r="I1">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="J1">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="K1">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="L1">
         <v>4</v>
       </c>
-      <c r="I1">
-        <v>0</v>
-      </c>
-      <c r="J1">
+      <c r="M1">
+        <v>5</v>
+      </c>
+      <c r="N1">
+        <v>6</v>
+      </c>
+      <c r="O1">
+        <v>7</v>
+      </c>
+      <c r="P1">
+        <v>8</v>
+      </c>
+      <c r="Q1">
+        <v>9</v>
+      </c>
+      <c r="R1">
+        <v>10</v>
+      </c>
+      <c r="S1">
+        <v>11</v>
+      </c>
+      <c r="T1">
+        <v>12</v>
+      </c>
+      <c r="U1">
+        <v>13</v>
+      </c>
+      <c r="V1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="K1">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="L1">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="M1">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="N1">
+      <c r="G2" t="s">
         <v>5</v>
       </c>
-      <c r="O1">
+      <c r="P2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3">
+        <v>10000</v>
+      </c>
+      <c r="B3">
+        <v>5.5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="P1">
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
         <v>7</v>
       </c>
-      <c r="Q1">
+      <c r="S3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4">
+        <v>20000</v>
+      </c>
+      <c r="B4">
+        <v>9.2</v>
+      </c>
+      <c r="C4">
+        <f>B4/B3</f>
+        <v>1.67272727272727</v>
+      </c>
+      <c r="D4">
+        <f>LOG(B4,2)/LOG(B3,2)</f>
+        <v>1.30177795426717</v>
+      </c>
+      <c r="G4" t="s">
         <v>8</v>
       </c>
-      <c r="R1">
+      <c r="M4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5">
+        <v>40000</v>
+      </c>
+      <c r="B5">
+        <v>17.3</v>
+      </c>
+      <c r="C5">
+        <f>B5/B4</f>
+        <v>1.8804347826087</v>
+      </c>
+      <c r="D5">
+        <f>LOG(B5,2)/LOG(B4,2)</f>
+        <v>1.28456291727464</v>
+      </c>
+      <c r="G5" t="s">
         <v>9</v>
       </c>
-      <c r="S1">
+      <c r="Q5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6">
+        <v>80000</v>
+      </c>
+      <c r="B6">
+        <v>46.4</v>
+      </c>
+      <c r="C6">
+        <f>B6/B5</f>
+        <v>2.68208092485549</v>
+      </c>
+      <c r="D6">
+        <f>LOG(B6,2)/LOG(B5,2)</f>
+        <v>1.34608717425244</v>
+      </c>
+      <c r="G6" t="s">
         <v>10</v>
       </c>
-      <c r="T1">
+      <c r="L6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>160000</v>
+      </c>
+      <c r="B7">
+        <v>78.2</v>
+      </c>
+      <c r="C7">
+        <f>B7/B6</f>
+        <v>1.68534482758621</v>
+      </c>
+      <c r="D7">
+        <f>LOG(B7,2)/LOG(B6,2)</f>
+        <v>1.13602539855555</v>
+      </c>
+      <c r="G7" t="s">
         <v>11</v>
       </c>
-      <c r="U1">
+      <c r="K7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>320000</v>
+      </c>
+      <c r="B8">
+        <v>193.2</v>
+      </c>
+      <c r="C8">
+        <f>B8/B7</f>
+        <v>2.47058823529412</v>
+      </c>
+      <c r="D8">
+        <f>LOG(B8,2)/LOG(B7,2)</f>
+        <v>1.20747885479743</v>
+      </c>
+      <c r="G8" t="s">
         <v>12</v>
       </c>
-      <c r="V1">
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>640000</v>
+      </c>
+      <c r="B9">
+        <v>394.5</v>
+      </c>
+      <c r="C9">
+        <f>B9/B8</f>
+        <v>2.04192546583851</v>
+      </c>
+      <c r="D9">
+        <f>LOG(B9,2)/LOG(B8,2)</f>
+        <v>1.1356250741616</v>
+      </c>
+      <c r="G9" t="s">
         <v>13</v>
       </c>
-      <c r="W1">
+      <c r="I9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10">
+        <v>1280000</v>
+      </c>
+      <c r="B10">
+        <v>1003.8</v>
+      </c>
+      <c r="C10">
+        <f>B10/B9</f>
+        <v>2.54448669201521</v>
+      </c>
+      <c r="D10">
+        <f>LOG(B10,2)/LOG(B9,2)</f>
+        <v>1.15623761149999</v>
+      </c>
+      <c r="G10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="8:17">
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q2">
+      <c r="H10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11">
+        <v>2560000</v>
+      </c>
+      <c r="B11">
+        <v>2882.2</v>
+      </c>
+      <c r="C11">
+        <f>B11/B10</f>
+        <v>2.87128910141462</v>
+      </c>
+      <c r="D11">
+        <f>LOG(B11,2)/LOG(B10,2)</f>
+        <v>1.15260851568981</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="T11">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="8:20">
-      <c r="H3" t="s">
-        <v>6</v>
-      </c>
-      <c r="T3">
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>5120000</v>
+      </c>
+      <c r="B12">
+        <v>8258.1</v>
+      </c>
+      <c r="C12">
+        <f>B12/B11</f>
+        <v>2.86520713343973</v>
+      </c>
+      <c r="D12">
+        <f>LOG(B12,2)/LOG(B11,2)</f>
+        <v>1.13213655444716</v>
+      </c>
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13">
+        <v>10240000</v>
+      </c>
+      <c r="B13">
+        <v>19882.1</v>
+      </c>
+      <c r="C13">
+        <f>B13/B12</f>
+        <v>2.40758770177159</v>
+      </c>
+      <c r="D13">
+        <f>LOG(B13,2)/LOG(B12,2)</f>
+        <v>1.09741991146783</v>
+      </c>
+      <c r="G13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="8:14">
-      <c r="H4" t="s">
-        <v>7</v>
-      </c>
-      <c r="N4">
+    <row r="14" spans="7:14">
+      <c r="G14" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="8:18">
-      <c r="H5" t="s">
-        <v>8</v>
-      </c>
-      <c r="R5">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="8:13">
-      <c r="H6" t="s">
-        <v>9</v>
-      </c>
-      <c r="M6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="8:12">
-      <c r="H7" t="s">
+    <row r="15" spans="7:7">
+      <c r="G15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="7:22">
+      <c r="G16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16">
         <v>10</v>
       </c>
-      <c r="L7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="8:8">
-      <c r="H8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="8:10">
-      <c r="H9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="8:9">
-      <c r="H10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10">
+      <c r="V16">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="8:21">
-      <c r="H11" t="s">
-        <v>14</v>
-      </c>
-      <c r="U11">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="8:8">
-      <c r="H12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="8:11">
-      <c r="H13" t="s">
-        <v>16</v>
-      </c>
-      <c r="K13">
+    <row r="17" spans="8:22">
+      <c r="H17">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="8:15">
-      <c r="H14" t="s">
-        <v>17</v>
-      </c>
-      <c r="O14">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="8:8">
-      <c r="H15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="8:23">
-      <c r="H16" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16">
-        <v>10</v>
-      </c>
-      <c r="W16">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="9:23">
       <c r="I17">
         <v>10</v>
       </c>
@@ -1331,201 +1517,370 @@
         <v>10</v>
       </c>
       <c r="K17">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="L17">
         <v>6</v>
       </c>
       <c r="M17">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="N17">
         <v>10</v>
       </c>
       <c r="O17">
+        <v>7</v>
+      </c>
+      <c r="P17">
+        <v>13</v>
+      </c>
+      <c r="Q17">
+        <v>14</v>
+      </c>
+      <c r="R17">
         <v>10</v>
-      </c>
-      <c r="P17">
-        <v>7</v>
-      </c>
-      <c r="Q17">
-        <v>13</v>
-      </c>
-      <c r="R17">
-        <v>14</v>
       </c>
       <c r="S17">
         <v>10</v>
       </c>
       <c r="T17">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="U17">
         <v>13</v>
       </c>
       <c r="V17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+      <c r="K19">
+        <v>3</v>
+      </c>
+      <c r="L19">
+        <v>4</v>
+      </c>
+      <c r="M19">
+        <v>5</v>
+      </c>
+      <c r="N19">
+        <v>6</v>
+      </c>
+      <c r="O19">
+        <v>7</v>
+      </c>
+      <c r="P19">
+        <v>8</v>
+      </c>
+      <c r="Q19">
+        <v>9</v>
+      </c>
+      <c r="R19">
+        <v>10</v>
+      </c>
+      <c r="S19">
+        <v>11</v>
+      </c>
+      <c r="T19">
+        <v>12</v>
+      </c>
+      <c r="U19">
         <v>13</v>
       </c>
-      <c r="W17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="9:23">
-      <c r="I19">
+      <c r="V19">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
+      <c r="A20">
+        <v>10000</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" t="s">
+        <v>22</v>
+      </c>
+      <c r="U20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21">
+        <v>20000</v>
+      </c>
+      <c r="B21">
+        <v>15.5</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ref="C21:C30" si="0">B21/B20</f>
+        <v>1.9375</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21:D30" si="1">LOG(B21,2)/LOG(B20,2)</f>
+        <v>1.31806543679563</v>
+      </c>
+      <c r="G21" t="s">
+        <v>23</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22">
+        <v>40000</v>
+      </c>
+      <c r="B22">
+        <v>18.7</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>1.20645161290323</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>1.06847663427892</v>
+      </c>
+      <c r="G22" t="s">
+        <v>24</v>
+      </c>
+      <c r="R22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23">
+        <v>80000</v>
+      </c>
+      <c r="B23">
+        <v>50.7</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>2.71122994652406</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>1.34058199587954</v>
+      </c>
+      <c r="G23" t="s">
+        <v>25</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24">
+        <v>160000</v>
+      </c>
+      <c r="B24">
+        <v>88.8</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>1.75147928994083</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>1.14275886814067</v>
+      </c>
+      <c r="G24" t="s">
+        <v>26</v>
+      </c>
+      <c r="T24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>320000</v>
+      </c>
+      <c r="B25">
+        <v>217.8</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>2.4527027027027</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>1.19998065938011</v>
+      </c>
+      <c r="G25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="A26">
+        <v>640000</v>
+      </c>
+      <c r="B26">
+        <v>466.5</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>2.14187327823691</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>1.14148228584948</v>
+      </c>
+      <c r="G26" t="s">
+        <v>12</v>
+      </c>
+      <c r="S26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>1280000</v>
+      </c>
+      <c r="B27">
+        <v>991.1</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>2.12454448017149</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>1.12262421116209</v>
+      </c>
+      <c r="G27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28">
+        <v>2560000</v>
+      </c>
+      <c r="B28">
+        <v>2958.9</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>2.98547068913329</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>1.1585427859519</v>
+      </c>
+      <c r="G28" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <v>5120000</v>
+      </c>
+      <c r="B29">
+        <v>10562.1</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>3.56960356889385</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>1.15920462250683</v>
+      </c>
+      <c r="G29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30">
+        <v>10240000</v>
+      </c>
+      <c r="B30">
+        <v>28685.3</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>2.71587089688604</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>1.10783699076397</v>
+      </c>
+      <c r="G30" t="s">
+        <v>29</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="7:21">
+      <c r="G31" t="s">
+        <v>30</v>
+      </c>
+      <c r="O31">
+        <v>1</v>
+      </c>
+      <c r="U31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="7:14">
+      <c r="G32" t="s">
+        <v>31</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="7:7">
+      <c r="G33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="7:22">
+      <c r="G34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H34">
         <v>0</v>
       </c>
-      <c r="J19">
+      <c r="I34">
         <v>1</v>
-      </c>
-      <c r="K19">
-        <v>2</v>
-      </c>
-      <c r="L19">
-        <v>3</v>
-      </c>
-      <c r="M19">
-        <v>4</v>
-      </c>
-      <c r="N19">
-        <v>5</v>
-      </c>
-      <c r="O19">
-        <v>6</v>
-      </c>
-      <c r="P19">
-        <v>7</v>
-      </c>
-      <c r="Q19">
-        <v>8</v>
-      </c>
-      <c r="R19">
-        <v>9</v>
-      </c>
-      <c r="S19">
-        <v>10</v>
-      </c>
-      <c r="T19">
-        <v>11</v>
-      </c>
-      <c r="U19">
-        <v>12</v>
-      </c>
-      <c r="V19">
-        <v>13</v>
-      </c>
-      <c r="W19">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="8:22">
-      <c r="H20" t="s">
-        <v>20</v>
-      </c>
-      <c r="V20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="8:17">
-      <c r="H21" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="8:19">
-      <c r="H22" t="s">
-        <v>22</v>
-      </c>
-      <c r="S22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="8:11">
-      <c r="H23" t="s">
-        <v>23</v>
-      </c>
-      <c r="K23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="8:21">
-      <c r="H24" t="s">
-        <v>24</v>
-      </c>
-      <c r="U24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="8:8">
-      <c r="H25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="8:20">
-      <c r="H26" t="s">
-        <v>11</v>
-      </c>
-      <c r="T26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="8:8">
-      <c r="H27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="8:18">
-      <c r="H28" t="s">
-        <v>26</v>
-      </c>
-      <c r="R28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="8:8">
-      <c r="H29" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="8:12">
-      <c r="H30" t="s">
-        <v>27</v>
-      </c>
-      <c r="L30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="8:22">
-      <c r="H31" t="s">
-        <v>28</v>
-      </c>
-      <c r="P31">
-        <v>1</v>
-      </c>
-      <c r="V31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="8:15">
-      <c r="H32" t="s">
-        <v>29</v>
-      </c>
-      <c r="O32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="8:8">
-      <c r="H33" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="8:23">
-      <c r="H34" t="s">
-        <v>31</v>
-      </c>
-      <c r="I34">
-        <v>0</v>
       </c>
       <c r="J34">
         <v>1</v>
@@ -1534,13 +1889,13 @@
         <v>1</v>
       </c>
       <c r="L34">
+        <v>4</v>
+      </c>
+      <c r="M34">
+        <v>5</v>
+      </c>
+      <c r="N34">
         <v>1</v>
-      </c>
-      <c r="M34">
-        <v>4</v>
-      </c>
-      <c r="N34">
-        <v>5</v>
       </c>
       <c r="O34">
         <v>1</v>
@@ -1552,128 +1907,128 @@
         <v>1</v>
       </c>
       <c r="R34">
+        <v>3</v>
+      </c>
+      <c r="S34">
+        <v>5</v>
+      </c>
+      <c r="T34">
         <v>1</v>
-      </c>
-      <c r="S34">
-        <v>3</v>
-      </c>
-      <c r="T34">
-        <v>5</v>
       </c>
       <c r="U34">
         <v>1</v>
       </c>
       <c r="V34">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="8:17">
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
         <v>1</v>
       </c>
-      <c r="W34">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="9:18">
-      <c r="I36">
-        <v>0</v>
-      </c>
       <c r="J36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K36">
+        <v>3</v>
+      </c>
+      <c r="L36">
+        <v>4</v>
+      </c>
+      <c r="M36">
+        <v>5</v>
+      </c>
+      <c r="N36">
+        <v>6</v>
+      </c>
+      <c r="O36">
+        <v>7</v>
+      </c>
+      <c r="P36">
+        <v>8</v>
+      </c>
+      <c r="Q36">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="7:16">
+      <c r="G37" t="s">
+        <v>34</v>
+      </c>
+      <c r="P37">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="7:7">
+      <c r="G38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="7:9">
+      <c r="G39" t="s">
+        <v>36</v>
+      </c>
+      <c r="I39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="7:8">
+      <c r="G40" t="s">
+        <v>37</v>
+      </c>
+      <c r="H40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="7:14">
+      <c r="G41" t="s">
+        <v>38</v>
+      </c>
+      <c r="N41">
         <v>2</v>
       </c>
-      <c r="L36">
-        <v>3</v>
-      </c>
-      <c r="M36">
+    </row>
+    <row r="42" spans="7:17">
+      <c r="G42" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q42">
         <v>4</v>
       </c>
-      <c r="N36">
-        <v>5</v>
-      </c>
-      <c r="O36">
-        <v>6</v>
-      </c>
-      <c r="P36">
-        <v>7</v>
-      </c>
-      <c r="Q36">
-        <v>8</v>
-      </c>
-      <c r="R36">
+    </row>
+    <row r="43" spans="7:7">
+      <c r="G43" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="7:15">
+      <c r="G44" t="s">
+        <v>41</v>
+      </c>
+      <c r="O44">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="8:17">
-      <c r="H37" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q37">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="8:8">
-      <c r="H38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="8:10">
-      <c r="H39" t="s">
-        <v>34</v>
-      </c>
-      <c r="J39">
+    <row r="45" spans="7:10">
+      <c r="G45" t="s">
+        <v>10</v>
+      </c>
+      <c r="J45">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="8:9">
-      <c r="H40" t="s">
-        <v>35</v>
-      </c>
-      <c r="I40">
+    <row r="46" spans="7:7">
+      <c r="G46" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="8:17">
+      <c r="H47">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="8:15">
-      <c r="H41" t="s">
-        <v>36</v>
-      </c>
-      <c r="O41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="8:18">
-      <c r="H42" t="s">
-        <v>37</v>
-      </c>
-      <c r="R42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="8:8">
-      <c r="H43" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="44" spans="8:16">
-      <c r="H44" t="s">
-        <v>39</v>
-      </c>
-      <c r="P44">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45" spans="8:11">
-      <c r="H45" t="s">
-        <v>9</v>
-      </c>
-      <c r="K45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="8:8">
-      <c r="H46" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="47" spans="9:18">
       <c r="I47">
         <v>4</v>
       </c>
@@ -1681,149 +2036,149 @@
         <v>4</v>
       </c>
       <c r="K47">
+        <v>3</v>
+      </c>
+      <c r="L47">
         <v>4</v>
       </c>
-      <c r="L47">
-        <v>3</v>
-      </c>
       <c r="M47">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O47">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="P47">
         <v>9</v>
       </c>
       <c r="Q47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="8:17">
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="J50">
+        <v>2</v>
+      </c>
+      <c r="K50">
+        <v>3</v>
+      </c>
+      <c r="L50">
+        <v>4</v>
+      </c>
+      <c r="M50">
+        <v>5</v>
+      </c>
+      <c r="N50">
+        <v>6</v>
+      </c>
+      <c r="O50">
+        <v>7</v>
+      </c>
+      <c r="P50">
+        <v>8</v>
+      </c>
+      <c r="Q50">
         <v>9</v>
       </c>
-      <c r="R47">
+    </row>
+    <row r="51" spans="7:13">
+      <c r="G51" t="s">
+        <v>43</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="7:9">
+      <c r="G52" t="s">
+        <v>44</v>
+      </c>
+      <c r="H52"/>
+      <c r="I52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="7:17">
+      <c r="G53" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q53">
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="9:18">
-      <c r="I50">
+    <row r="54" spans="7:10">
+      <c r="G54" t="s">
+        <v>46</v>
+      </c>
+      <c r="J54">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="7:11">
+      <c r="G55" t="s">
+        <v>47</v>
+      </c>
+      <c r="K55">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="7:14">
+      <c r="G56" t="s">
+        <v>48</v>
+      </c>
+      <c r="N56">
         <v>0</v>
       </c>
-      <c r="J50">
-        <v>1</v>
-      </c>
-      <c r="K50">
-        <v>2</v>
-      </c>
-      <c r="L50">
-        <v>3</v>
-      </c>
-      <c r="M50">
-        <v>4</v>
-      </c>
-      <c r="N50">
-        <v>5</v>
-      </c>
-      <c r="O50">
-        <v>6</v>
-      </c>
-      <c r="P50">
-        <v>7</v>
-      </c>
-      <c r="Q50">
-        <v>8</v>
-      </c>
-      <c r="R50">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="8:14">
-      <c r="H51" t="s">
-        <v>41</v>
-      </c>
-      <c r="N51">
+    </row>
+    <row r="57" spans="7:15">
+      <c r="G57" t="s">
+        <v>49</v>
+      </c>
+      <c r="O57">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="8:10">
-      <c r="H52" t="s">
-        <v>42</v>
-      </c>
-      <c r="I52"/>
-      <c r="J52">
+    <row r="58" spans="7:12">
+      <c r="G58" t="s">
+        <v>50</v>
+      </c>
+      <c r="L58">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="8:18">
-      <c r="H53" t="s">
-        <v>43</v>
-      </c>
-      <c r="R53">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="8:11">
-      <c r="H54" t="s">
-        <v>44</v>
-      </c>
-      <c r="K54">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="8:12">
-      <c r="H55" t="s">
-        <v>45</v>
-      </c>
-      <c r="L55">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="8:15">
-      <c r="H56" t="s">
-        <v>46</v>
-      </c>
-      <c r="O56">
+    <row r="59" spans="7:7">
+      <c r="G59" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="7:7">
+      <c r="G60" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="8:17">
+      <c r="H61">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="8:16">
-      <c r="H57" t="s">
-        <v>47</v>
-      </c>
-      <c r="P57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="8:13">
-      <c r="H58" t="s">
-        <v>48</v>
-      </c>
-      <c r="M58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="8:8">
-      <c r="H59" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="60" spans="8:8">
-      <c r="H60" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="61" spans="9:18">
       <c r="I61">
         <v>0</v>
       </c>
       <c r="J61">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K61">
         <v>6</v>
       </c>
       <c r="L61">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="M61">
         <v>0</v>
@@ -1835,135 +2190,261 @@
         <v>0</v>
       </c>
       <c r="P61">
+        <v>8</v>
+      </c>
+      <c r="Q61">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="8:22">
+      <c r="H64">
         <v>0</v>
       </c>
-      <c r="Q61">
+      <c r="I64">
+        <v>1</v>
+      </c>
+      <c r="J64">
+        <v>2</v>
+      </c>
+      <c r="K64">
+        <v>3</v>
+      </c>
+      <c r="L64">
+        <v>4</v>
+      </c>
+      <c r="M64">
+        <v>5</v>
+      </c>
+      <c r="N64">
+        <v>6</v>
+      </c>
+      <c r="O64">
+        <v>7</v>
+      </c>
+      <c r="P64">
         <v>8</v>
       </c>
-      <c r="R61">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="63" spans="9:23">
-      <c r="I63">
-        <v>0</v>
-      </c>
-      <c r="J63">
-        <v>1</v>
-      </c>
-      <c r="K63">
+      <c r="Q64">
+        <v>9</v>
+      </c>
+      <c r="R64">
+        <v>10</v>
+      </c>
+      <c r="S64">
+        <v>11</v>
+      </c>
+      <c r="T64">
+        <v>12</v>
+      </c>
+      <c r="U64">
+        <v>13</v>
+      </c>
+      <c r="V64">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="7:20">
+      <c r="G65" t="s">
+        <v>19</v>
+      </c>
+      <c r="T65">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="7:11">
+      <c r="G66" t="s">
+        <v>47</v>
+      </c>
+      <c r="K66">
         <v>2</v>
       </c>
-      <c r="L63">
-        <v>3</v>
-      </c>
-      <c r="M63">
-        <v>4</v>
-      </c>
-      <c r="N63">
+    </row>
+    <row r="67" spans="7:7">
+      <c r="G67" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="68" spans="7:12">
+      <c r="G68" t="s">
+        <v>54</v>
+      </c>
+      <c r="L68">
         <v>5</v>
       </c>
-      <c r="O63">
+    </row>
+    <row r="69" spans="7:16">
+      <c r="G69" t="s">
+        <v>55</v>
+      </c>
+      <c r="P69">
         <v>6</v>
       </c>
-      <c r="P63">
-        <v>7</v>
-      </c>
-      <c r="Q63">
-        <v>8</v>
-      </c>
-      <c r="R63">
-        <v>9</v>
-      </c>
-      <c r="S63">
-        <v>10</v>
-      </c>
-      <c r="T63">
-        <v>11</v>
-      </c>
-      <c r="U63">
-        <v>12</v>
-      </c>
-      <c r="V63">
+    </row>
+    <row r="70" spans="7:22">
+      <c r="G70" t="s">
+        <v>56</v>
+      </c>
+      <c r="V70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="7:14">
+      <c r="G71" t="s">
+        <v>52</v>
+      </c>
+      <c r="N71">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="7:8">
+      <c r="G72" t="s">
+        <v>57</v>
+      </c>
+      <c r="H72">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="7:19">
+      <c r="G73" t="s">
+        <v>58</v>
+      </c>
+      <c r="S73">
         <v>13</v>
       </c>
-      <c r="W63">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="64" spans="8:8">
-      <c r="H64" t="s">
+    </row>
+    <row r="74" spans="7:15">
+      <c r="G74" t="s">
+        <v>30</v>
+      </c>
+      <c r="O74">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75" spans="7:7">
+      <c r="G75" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="76" spans="7:17">
+      <c r="G76" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q76">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77" spans="7:21">
+      <c r="G77" t="s">
+        <v>60</v>
+      </c>
+      <c r="U77">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="7:10">
+      <c r="G78" t="s">
+        <v>61</v>
+      </c>
+      <c r="J78">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="7:7">
+      <c r="G79" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="80" spans="7:7">
+      <c r="G80" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="81" spans="7:7">
+      <c r="G81" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="82" spans="7:18">
+      <c r="G82" t="s">
+        <v>65</v>
+      </c>
+      <c r="R82">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="7:7">
+      <c r="G83" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="84" spans="7:7">
+      <c r="G84" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="85" spans="7:7">
+      <c r="G85" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="86" spans="7:7">
+      <c r="G86" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="87" spans="7:9">
+      <c r="G87" t="s">
+        <v>68</v>
+      </c>
+      <c r="I87">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="8:22">
+      <c r="H88">
+        <v>5</v>
+      </c>
+      <c r="I88">
+        <v>5</v>
+      </c>
+      <c r="J88">
+        <v>5</v>
+      </c>
+      <c r="K88">
+        <v>2</v>
+      </c>
+      <c r="L88">
+        <v>5</v>
+      </c>
+      <c r="M88">
+        <v>5</v>
+      </c>
+      <c r="N88">
+        <v>5</v>
+      </c>
+      <c r="O88">
+        <v>13</v>
+      </c>
+      <c r="P88">
         <v>6</v>
       </c>
-    </row>
-    <row r="65" spans="8:8">
-      <c r="H65" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="66" spans="8:8">
-      <c r="H66" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="67" spans="8:8">
-      <c r="H67" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="68" spans="8:8">
-      <c r="H68" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="69" spans="8:8">
-      <c r="H69" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="70" spans="8:8">
-      <c r="H70" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="71" spans="8:8">
-      <c r="H71" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="72" spans="8:8">
-      <c r="H72" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="73" spans="8:8">
-      <c r="H73" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="74" spans="8:8">
-      <c r="H74" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="75" spans="8:8">
-      <c r="H75" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="76" spans="8:8">
-      <c r="H76" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="77" spans="8:8">
-      <c r="H77" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="78" spans="8:8">
-      <c r="H78" t="s">
-        <v>9</v>
+      <c r="Q88">
+        <v>13</v>
+      </c>
+      <c r="R88">
+        <v>5</v>
+      </c>
+      <c r="S88">
+        <v>13</v>
+      </c>
+      <c r="T88">
+        <v>13</v>
+      </c>
+      <c r="U88">
+        <v>5</v>
+      </c>
+      <c r="V88">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>